<commit_message>
get bean from file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRacy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE70BA0A-976E-4D83-AA8F-4EAE4FEC28B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9C6142-00F1-4980-95B5-5AADDAB8BCD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>教师号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,51 +71,70 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>职称获取时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>博士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清华大学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>党员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机科学学院</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2010110155</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1975-10-25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2005-10-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2010110156</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1975-10-26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2005-10-11</t>
+  </si>
+  <si>
+    <t>女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周福山</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李敏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>职称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职称获取时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>张三</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>男</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>博士</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>清华大学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>党员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>计算机科学学院</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2010110155</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1975-10-25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2005-10-10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -442,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -488,48 +507,86 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
         <v>123456</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
       </c>
       <c r="I2" s="1">
         <v>2010</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1">
+        <v>123456</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2011</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>